<commit_message>
new simulated data files, Reelin updated, model_characteristics.xlsx updated
</commit_message>
<xml_diff>
--- a/Benchmark-Models/Hass_PONE2017/Data/model1_data1.xlsx
+++ b/Benchmark-Models/Hass_PONE2017/Data/model1_data1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="20">
   <si>
     <t>time</t>
   </si>
@@ -990,16 +990,16 @@
         <v>-30.0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6034791370529051</v>
+        <v>0.6034918556212381</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04074057619458317</v>
+        <v>0.04067750374608078</v>
       </c>
       <c r="E2" t="n">
-        <v>0.24588895597661428</v>
+        <v>0.2458973248837802</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -1013,22 +1013,22 @@
         <v>0.0</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6034791370529051</v>
+        <v>0.6034918556212381</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.7724510352262276</v>
+        <v>-0.7724296443576986</v>
       </c>
       <c r="D3" t="n">
-        <v>0.04074057619458317</v>
+        <v>0.04067750374608078</v>
       </c>
       <c r="E3" t="n">
-        <v>0.24588895597661428</v>
+        <v>0.2458973248837802</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4984132392820122</v>
+        <v>0.4984118450512706</v>
       </c>
     </row>
     <row r="4">
@@ -1036,22 +1036,22 @@
         <v>1.0</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5998999034569327</v>
+        <v>0.5999191328171226</v>
       </c>
       <c r="C4" t="n">
-        <v>0.25496198354583766</v>
+        <v>0.25507219206275206</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3647339014412329</v>
+        <v>0.3648153051922902</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4603369677981738</v>
+        <v>0.46036663552237284</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.028341818789590682</v>
+        <v>-0.028338715746927187</v>
       </c>
       <c r="G4" t="n">
-        <v>0.49727147267115873</v>
+        <v>0.49727221828411877</v>
       </c>
     </row>
     <row r="5">
@@ -1059,22 +1059,22 @@
         <v>2.0</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5951480344499419</v>
+        <v>0.5951668360469289</v>
       </c>
       <c r="C5" t="n">
-        <v>0.28420476903814895</v>
+        <v>0.2841643140478611</v>
       </c>
       <c r="D5" t="n">
-        <v>0.38194015217864563</v>
+        <v>0.3819363667975573</v>
       </c>
       <c r="E5" t="n">
-        <v>0.45820857400687803</v>
+        <v>0.4582028524653246</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4957655214399496</v>
+        <v>0.49576620767666113</v>
       </c>
     </row>
     <row r="6">
@@ -1082,22 +1082,22 @@
         <v>3.0</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5903942701695043</v>
+        <v>0.5904126039841993</v>
       </c>
       <c r="C6" t="n">
-        <v>0.30822055888360295</v>
+        <v>0.3080837001722125</v>
       </c>
       <c r="D6" t="n">
-        <v>0.39642551673003334</v>
+        <v>0.3963647672051821</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4564241790443114</v>
+        <v>0.4564189299728072</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.028341818789704376</v>
+        <v>-0.028338715746908247</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4942702091225672</v>
+        <v>0.4942708251873052</v>
       </c>
     </row>
     <row r="7">
@@ -1105,22 +1105,22 @@
         <v>5.0</v>
       </c>
       <c r="B7" t="n">
-        <v>0.5808829363027711</v>
+        <v>0.5809002870751893</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3442011612461596</v>
+        <v>0.34394178498771566</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4187176560643093</v>
+        <v>0.4185806176662539</v>
       </c>
       <c r="E7" t="n">
-        <v>0.45285529940879804</v>
+        <v>0.4528506540223837</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.0283418187897998</v>
+        <v>-0.02833871574692266</v>
       </c>
       <c r="G7" t="n">
-        <v>0.49131195270274247</v>
+        <v>0.49131241947814625</v>
       </c>
     </row>
     <row r="8">
@@ -1128,22 +1128,22 @@
         <v>10.0</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5570963869462185</v>
+        <v>0.5571111133790713</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3899777807251886</v>
+        <v>0.38962763045757115</v>
       </c>
       <c r="D8" t="n">
-        <v>0.44808192700810273</v>
+        <v>0.4478836060295819</v>
       </c>
       <c r="E8" t="n">
-        <v>0.44398226894964865</v>
+        <v>0.443977961339434</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
       </c>
       <c r="G8" t="n">
-        <v>0.48410752149500424</v>
+        <v>0.48410759975657436</v>
       </c>
     </row>
     <row r="9">
@@ -1151,22 +1151,22 @@
         <v>15.0</v>
       </c>
       <c r="B9" t="n">
-        <v>0.5333218522107862</v>
+        <v>0.5333338556572826</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4006143257965234</v>
+        <v>0.40031276567190943</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4550626124753605</v>
+        <v>0.4548953616677865</v>
       </c>
       <c r="E9" t="n">
-        <v>0.4352528094276134</v>
+        <v>0.43524819924429925</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.02834181878977144</v>
+        <v>-0.02833871574695951</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4771785824237441</v>
+        <v>0.47717829452409843</v>
       </c>
     </row>
     <row r="10">
@@ -1174,22 +1174,22 @@
         <v>30.0</v>
       </c>
       <c r="B10" t="n">
-        <v>0.46227768298168276</v>
+        <v>0.46228133383123965</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3473349123467068</v>
+        <v>0.34738752420642194</v>
       </c>
       <c r="D10" t="n">
-        <v>0.42069233109017246</v>
+        <v>0.4207520246247629</v>
       </c>
       <c r="E10" t="n">
-        <v>0.41038278577164744</v>
+        <v>0.41037753011832717</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.028341818789632375</v>
+        <v>-0.02833871574691113</v>
       </c>
       <c r="G10" t="n">
-        <v>0.45803111474307034</v>
+        <v>0.45802996972124554</v>
       </c>
     </row>
     <row r="11">
@@ -1197,22 +1197,22 @@
         <v>45.0</v>
       </c>
       <c r="B11" t="n">
-        <v>0.39196395435191955</v>
+        <v>0.391958802511523</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2508479798936462</v>
+        <v>0.25120933163635617</v>
       </c>
       <c r="D11" t="n">
-        <v>0.36235160664166355</v>
+        <v>0.36257754210955595</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3878501286788226</v>
+        <v>0.3878452002625733</v>
       </c>
       <c r="F11" t="s">
         <v>19</v>
       </c>
       <c r="G11" t="n">
-        <v>0.44124661852887215</v>
+        <v>0.44124489782287757</v>
       </c>
     </row>
     <row r="12">
@@ -1220,22 +1220,22 @@
         <v>60.0</v>
       </c>
       <c r="B12" t="n">
-        <v>0.3227045011909161</v>
+        <v>0.3226899571563182</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1479012566259999</v>
+        <v>0.14841721366197386</v>
       </c>
       <c r="D12" t="n">
-        <v>0.30586345670595944</v>
+        <v>0.3061380936602115</v>
       </c>
       <c r="E12" t="n">
-        <v>0.36776196832093383</v>
+        <v>0.36775744151976436</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.028341818789634845</v>
+        <v>-0.02833871574681602</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4266502931381673</v>
+        <v>0.42664820952412275</v>
       </c>
     </row>
     <row r="13">
@@ -1243,22 +1243,22 @@
         <v>120.0</v>
       </c>
       <c r="B13" t="n">
-        <v>0.06189555437703978</v>
+        <v>0.06184421455362599</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.18680325287846242</v>
+        <v>-0.1865579619191787</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1637904353522499</v>
+        <v>0.163845627742501</v>
       </c>
       <c r="E13" t="n">
-        <v>0.30960214015181103</v>
+        <v>0.30959729056113167</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.028341818789619968</v>
+        <v>-0.028338715746792652</v>
       </c>
       <c r="G13" t="n">
-        <v>0.386046999076692</v>
+        <v>0.38604570249178094</v>
       </c>
     </row>
     <row r="14">
@@ -1266,22 +1266,22 @@
         <v>240.0</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.3291432787210932</v>
+        <v>-0.3291931794046952</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.5135751511567704</v>
+        <v>-0.5138572064124289</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0796038720077284</v>
+        <v>0.07949808036059004</v>
       </c>
       <c r="E14" t="n">
-        <v>0.26166978022619597</v>
+        <v>0.2616692742575686</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.028341818789691716</v>
+        <v>-0.028338715746721626</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3542138175040771</v>
+        <v>0.3542194635877747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>